<commit_message>
Quizz - Działający limit czasu, zmieniony wygląd
</commit_message>
<xml_diff>
--- a/Ardeno/Helpers/Lotrle.xlsx
+++ b/Ardeno/Helpers/Lotrle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Repozytorium GIT\Ardeno\Ardeno\Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD75CA0D-8B5F-4FE3-949B-1FCDBFE24032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327AE94F-A0FD-4124-8AF3-276089463C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -889,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:B177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C177"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,1420 +900,1419 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>166</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>74</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>75</v>
       </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>76</v>
       </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="C81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>81</v>
       </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="C88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="C89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="C90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="C92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="C93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="C95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="C99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="C100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-      <c r="C101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="C102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-      <c r="C103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>103</v>
       </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="C108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="C112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-      <c r="C113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>112</v>
       </c>
-      <c r="C114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-      <c r="C115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>114</v>
       </c>
-      <c r="C116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>115</v>
       </c>
-      <c r="C117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="C118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-      <c r="C119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="C120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>119</v>
       </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>120</v>
       </c>
-      <c r="C122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>121</v>
       </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>122</v>
       </c>
-      <c r="C124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>123</v>
       </c>
-      <c r="C125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>124</v>
       </c>
-      <c r="C126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>125</v>
       </c>
-      <c r="C127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>126</v>
       </c>
-      <c r="C128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>127</v>
       </c>
-      <c r="C129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>128</v>
       </c>
-      <c r="C130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>129</v>
       </c>
-      <c r="C131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>130</v>
       </c>
-      <c r="C132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>131</v>
       </c>
-      <c r="C133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>132</v>
       </c>
-      <c r="C134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-      <c r="C135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>134</v>
       </c>
-      <c r="C136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>135</v>
       </c>
-      <c r="C137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>136</v>
       </c>
-      <c r="C138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>137</v>
       </c>
-      <c r="C139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>138</v>
       </c>
-      <c r="C140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>139</v>
       </c>
-      <c r="C141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>140</v>
       </c>
-      <c r="C142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>141</v>
       </c>
-      <c r="C143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>142</v>
       </c>
-      <c r="C144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>143</v>
       </c>
-      <c r="C145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>144</v>
       </c>
-      <c r="C146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>145</v>
       </c>
-      <c r="C147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>146</v>
       </c>
-      <c r="C148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>147</v>
       </c>
-      <c r="C149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>148</v>
       </c>
-      <c r="C150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>149</v>
       </c>
-      <c r="C151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>150</v>
       </c>
-      <c r="C152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>151</v>
       </c>
-      <c r="C153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>152</v>
       </c>
-      <c r="C154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>153</v>
       </c>
-      <c r="C155">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>154</v>
       </c>
-      <c r="C156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>155</v>
       </c>
-      <c r="C157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>156</v>
       </c>
-      <c r="C158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>157</v>
       </c>
-      <c r="C159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>158</v>
       </c>
-      <c r="C160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>159</v>
       </c>
-      <c r="C161">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>160</v>
       </c>
-      <c r="C162">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>161</v>
       </c>
-      <c r="C163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>162</v>
       </c>
-      <c r="C164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>163</v>
       </c>
-      <c r="C165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>164</v>
       </c>
-      <c r="C166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="C167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>167</v>
       </c>
-      <c r="C168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>168</v>
       </c>
-      <c r="C169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>169</v>
       </c>
-      <c r="C170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>170</v>
       </c>
-      <c r="C171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>171</v>
       </c>
-      <c r="C172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>172</v>
       </c>
-      <c r="C173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>173</v>
       </c>
-      <c r="C174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>174</v>
       </c>
-      <c r="C175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>175</v>
       </c>
-      <c r="C176">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>176</v>
       </c>
-      <c r="C177">
+      <c r="B177">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Cleanup | Poprawki Animacji | Cytaty | Usuwanie niepotrzebnego kodu
</commit_message>
<xml_diff>
--- a/Ardeno/Helpers/Lotrle.xlsx
+++ b/Ardeno/Helpers/Lotrle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Repozytorium GIT\Ardeno\Ardeno\Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC371005-B838-4E30-972B-AC5885595238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68D6E60-10F4-44D2-89ED-2AF673E8545D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10092" yWindow="2280" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="274">
   <si>
     <t>Legolas</t>
   </si>
@@ -754,6 +754,99 @@
   </si>
   <si>
     <t>Niebieski Istari.</t>
+  </si>
+  <si>
+    <t>Jeden z pięciu Istarich</t>
+  </si>
+  <si>
+    <t>Pierwsze imię Sarumana</t>
+  </si>
+  <si>
+    <t>Jedno z wielu imion Gandalfa</t>
+  </si>
+  <si>
+    <t>Imię tego króla pochodziło od niesamowitego talentu</t>
+  </si>
+  <si>
+    <t>Zginął w Ostatnim Sojuszu Ludzi i Elfów.</t>
+  </si>
+  <si>
+    <t>Jego ród był przeklęty.</t>
+  </si>
+  <si>
+    <t>Huan</t>
+  </si>
+  <si>
+    <t>Ogromny pies.</t>
+  </si>
+  <si>
+    <t>"Gadzi język"</t>
+  </si>
+  <si>
+    <t>Nie umiał w zagadki.</t>
+  </si>
+  <si>
+    <t>Niedoceniany przez ojca, który oparł się Pierścieniowi.</t>
+  </si>
+  <si>
+    <t>Jej śpiew usypiał.</t>
+  </si>
+  <si>
+    <t>Czarnoksiężnik go niedocenił.</t>
+  </si>
+  <si>
+    <t>Mędrzec czy głupiec?</t>
+  </si>
+  <si>
+    <t>Ungolianta czy to ty?</t>
+  </si>
+  <si>
+    <t>Był tam jeden z Palantirów.</t>
+  </si>
+  <si>
+    <t>Jego własny włamywacz go okradł</t>
+  </si>
+  <si>
+    <t>Berło.</t>
+  </si>
+  <si>
+    <t>Mroczna Puszcza.</t>
+  </si>
+  <si>
+    <t>Miał kształt gwiazdy.</t>
+  </si>
+  <si>
+    <t>Królestwo Południa.</t>
+  </si>
+  <si>
+    <t>Planeta.</t>
+  </si>
+  <si>
+    <t>Miasto tysiąca jaskiń</t>
+  </si>
+  <si>
+    <t>Miasto zniszczone przez smoka czy bardziej przez pechowca?</t>
+  </si>
+  <si>
+    <t>Czy ten balrog mocno śpi? Sprawdźmy</t>
+  </si>
+  <si>
+    <t>Pierścień władzy.</t>
+  </si>
+  <si>
+    <t>Wzgórze Tuna.</t>
+  </si>
+  <si>
+    <t>Pierwsze bratobójstwo.</t>
+  </si>
+  <si>
+    <t>To statki mogą latać?</t>
+  </si>
+  <si>
+    <t>Stwórca.</t>
+  </si>
+  <si>
+    <t>Głupi Tuk?</t>
   </si>
 </sst>
 </file>
@@ -1096,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="B178" sqref="B178"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1332,6 +1425,9 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>253</v>
+      </c>
       <c r="C21">
         <v>0</v>
       </c>
@@ -1436,6 +1532,9 @@
       <c r="A31" t="s">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>252</v>
+      </c>
       <c r="C31">
         <v>0</v>
       </c>
@@ -1444,6 +1543,9 @@
       <c r="A32" t="s">
         <v>31</v>
       </c>
+      <c r="B32" t="s">
+        <v>251</v>
+      </c>
       <c r="C32">
         <v>0</v>
       </c>
@@ -1463,6 +1565,9 @@
       <c r="A34" t="s">
         <v>33</v>
       </c>
+      <c r="B34" t="s">
+        <v>248</v>
+      </c>
       <c r="C34">
         <v>0</v>
       </c>
@@ -1493,6 +1598,9 @@
       <c r="A37" t="s">
         <v>36</v>
       </c>
+      <c r="B37" t="s">
+        <v>254</v>
+      </c>
       <c r="C37">
         <v>0</v>
       </c>
@@ -1539,6 +1647,9 @@
       <c r="A42" t="s">
         <v>41</v>
       </c>
+      <c r="B42" t="s">
+        <v>255</v>
+      </c>
       <c r="C42">
         <v>0</v>
       </c>
@@ -1599,6 +1710,9 @@
       <c r="A48" t="s">
         <v>47</v>
       </c>
+      <c r="B48" t="s">
+        <v>256</v>
+      </c>
       <c r="C48">
         <v>0</v>
       </c>
@@ -1618,6 +1732,9 @@
       <c r="A50" t="s">
         <v>48</v>
       </c>
+      <c r="B50" t="s">
+        <v>257</v>
+      </c>
       <c r="C50">
         <v>0</v>
       </c>
@@ -1670,6 +1787,9 @@
       <c r="A55" t="s">
         <v>53</v>
       </c>
+      <c r="B55" t="s">
+        <v>258</v>
+      </c>
       <c r="C55">
         <v>0</v>
       </c>
@@ -1689,6 +1809,9 @@
       <c r="A57" t="s">
         <v>55</v>
       </c>
+      <c r="B57" t="s">
+        <v>259</v>
+      </c>
       <c r="C57">
         <v>0</v>
       </c>
@@ -2130,6 +2253,9 @@
       <c r="A105" t="s">
         <v>103</v>
       </c>
+      <c r="B105" t="s">
+        <v>260</v>
+      </c>
       <c r="C105">
         <v>0</v>
       </c>
@@ -2162,6 +2288,9 @@
       <c r="A109" t="s">
         <v>107</v>
       </c>
+      <c r="B109" t="s">
+        <v>261</v>
+      </c>
       <c r="C109">
         <v>0</v>
       </c>
@@ -2202,6 +2331,9 @@
       <c r="A114" t="s">
         <v>112</v>
       </c>
+      <c r="B114" t="s">
+        <v>262</v>
+      </c>
       <c r="C114">
         <v>0</v>
       </c>
@@ -2250,6 +2382,9 @@
       <c r="A120" t="s">
         <v>118</v>
       </c>
+      <c r="B120" t="s">
+        <v>263</v>
+      </c>
       <c r="C120">
         <v>0</v>
       </c>
@@ -2258,6 +2393,9 @@
       <c r="A121" t="s">
         <v>119</v>
       </c>
+      <c r="B121" t="s">
+        <v>264</v>
+      </c>
       <c r="C121">
         <v>0</v>
       </c>
@@ -2274,6 +2412,9 @@
       <c r="A123" t="s">
         <v>121</v>
       </c>
+      <c r="B123" t="s">
+        <v>265</v>
+      </c>
       <c r="C123">
         <v>0</v>
       </c>
@@ -2290,6 +2431,9 @@
       <c r="A125" t="s">
         <v>123</v>
       </c>
+      <c r="B125" t="s">
+        <v>266</v>
+      </c>
       <c r="C125">
         <v>0</v>
       </c>
@@ -2338,6 +2482,9 @@
       <c r="A131" t="s">
         <v>129</v>
       </c>
+      <c r="B131" t="s">
+        <v>267</v>
+      </c>
       <c r="C131">
         <v>0</v>
       </c>
@@ -2354,6 +2501,9 @@
       <c r="A133" t="s">
         <v>131</v>
       </c>
+      <c r="B133" t="s">
+        <v>268</v>
+      </c>
       <c r="C133">
         <v>0</v>
       </c>
@@ -2418,6 +2568,9 @@
       <c r="A141" t="s">
         <v>139</v>
       </c>
+      <c r="B141" t="s">
+        <v>269</v>
+      </c>
       <c r="C141">
         <v>0</v>
       </c>
@@ -2426,6 +2579,9 @@
       <c r="A142" t="s">
         <v>140</v>
       </c>
+      <c r="B142" t="s">
+        <v>270</v>
+      </c>
       <c r="C142">
         <v>0</v>
       </c>
@@ -2482,6 +2638,9 @@
       <c r="A149" t="s">
         <v>147</v>
       </c>
+      <c r="B149" t="s">
+        <v>271</v>
+      </c>
       <c r="C149">
         <v>0</v>
       </c>
@@ -2522,6 +2681,9 @@
       <c r="A154" t="s">
         <v>152</v>
       </c>
+      <c r="B154" t="s">
+        <v>273</v>
+      </c>
       <c r="C154">
         <v>0</v>
       </c>
@@ -2538,6 +2700,9 @@
       <c r="A156" t="s">
         <v>154</v>
       </c>
+      <c r="B156" t="s">
+        <v>272</v>
+      </c>
       <c r="C156">
         <v>0</v>
       </c>
@@ -2626,6 +2791,9 @@
       <c r="A167" t="s">
         <v>166</v>
       </c>
+      <c r="B167" t="s">
+        <v>247</v>
+      </c>
       <c r="C167">
         <v>0</v>
       </c>
@@ -2666,6 +2834,9 @@
       <c r="A172" t="s">
         <v>171</v>
       </c>
+      <c r="B172" t="s">
+        <v>246</v>
+      </c>
       <c r="C172">
         <v>0</v>
       </c>
@@ -2693,6 +2864,9 @@
       <c r="A175" t="s">
         <v>174</v>
       </c>
+      <c r="B175" t="s">
+        <v>245</v>
+      </c>
       <c r="C175">
         <v>0</v>
       </c>
@@ -2701,6 +2875,9 @@
       <c r="A176" t="s">
         <v>175</v>
       </c>
+      <c r="B176" t="s">
+        <v>244</v>
+      </c>
       <c r="C176">
         <v>0</v>
       </c>
@@ -2709,6 +2886,9 @@
       <c r="A177" t="s">
         <v>231</v>
       </c>
+      <c r="B177" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
@@ -2716,6 +2896,14 @@
       </c>
       <c r="B178" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>249</v>
+      </c>
+      <c r="B179" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rozdzielenie przycisków czyszczenia db i dodawania rekordów | zmiany wyglądu
</commit_message>
<xml_diff>
--- a/Ardeno/Helpers/Lotrle.xlsx
+++ b/Ardeno/Helpers/Lotrle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Repozytorium GIT\Ardeno\Ardeno\Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68D6E60-10F4-44D2-89ED-2AF673E8545D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF0025D-8EB5-48F2-B0AB-E951F14313E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10872" yWindow="4380" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="334">
   <si>
     <t>Legolas</t>
   </si>
@@ -306,9 +306,6 @@
     <t>Finduilas</t>
   </si>
   <si>
-    <t>Orodreth</t>
-  </si>
-  <si>
     <t>Dior</t>
   </si>
   <si>
@@ -327,9 +324,6 @@
     <t>ArPharazon</t>
   </si>
   <si>
-    <t>TarMiriel</t>
-  </si>
-  <si>
     <t>Azog</t>
   </si>
   <si>
@@ -345,9 +339,6 @@
     <t>MinasMorgul</t>
   </si>
   <si>
-    <t>Eriador</t>
-  </si>
-  <si>
     <t>Rhovanion</t>
   </si>
   <si>
@@ -459,9 +450,6 @@
     <t>Esgaroth</t>
   </si>
   <si>
-    <t>Vinyamar</t>
-  </si>
-  <si>
     <t>Fornost</t>
   </si>
   <si>
@@ -477,45 +465,21 @@
     <t>Turgon</t>
   </si>
   <si>
-    <t>Nori</t>
-  </si>
-  <si>
     <t>Bombur</t>
   </si>
   <si>
     <t>Pippin</t>
   </si>
   <si>
-    <t>Gloin</t>
-  </si>
-  <si>
     <t>EruIluvatar</t>
   </si>
   <si>
-    <t>Dwalin</t>
-  </si>
-  <si>
-    <t>Dori</t>
-  </si>
-  <si>
     <t>Ori</t>
   </si>
   <si>
-    <t>Oin</t>
-  </si>
-  <si>
-    <t>Bifur</t>
-  </si>
-  <si>
-    <t>Bofur</t>
-  </si>
-  <si>
     <t>Dain</t>
   </si>
   <si>
-    <t>Thror</t>
-  </si>
-  <si>
     <t>Thrain</t>
   </si>
   <si>
@@ -528,9 +492,6 @@
     <t>Anarion</t>
   </si>
   <si>
-    <t>Imrahil</t>
-  </si>
-  <si>
     <t>TarElendil</t>
   </si>
   <si>
@@ -660,9 +621,6 @@
     <t>Najsilniejszy Ainur.</t>
   </si>
   <si>
-    <t>Żelazna Dom</t>
-  </si>
-  <si>
     <t>Inne imię Króla Sindarów</t>
   </si>
   <si>
@@ -834,9 +792,6 @@
     <t>Pierścień władzy.</t>
   </si>
   <si>
-    <t>Wzgórze Tuna.</t>
-  </si>
-  <si>
     <t>Pierwsze bratobójstwo.</t>
   </si>
   <si>
@@ -847,6 +802,231 @@
   </si>
   <si>
     <t>Głupi Tuk?</t>
+  </si>
+  <si>
+    <t>Syn Barahira.</t>
+  </si>
+  <si>
+    <t>Opiekował się Elrondem i Elrosem.</t>
+  </si>
+  <si>
+    <t>Wilkołak.</t>
+  </si>
+  <si>
+    <t>Odrzuciła Maeglina.</t>
+  </si>
+  <si>
+    <t>Przez przekleństwo Morgortha jego życie było pamem nieszczęść.</t>
+  </si>
+  <si>
+    <t>Wędrował długie lata.</t>
+  </si>
+  <si>
+    <t>Siostra Yavanny.</t>
+  </si>
+  <si>
+    <t>Rozpętuje sztormy na morzu.</t>
+  </si>
+  <si>
+    <t>Jedno z drzew Valinoru.</t>
+  </si>
+  <si>
+    <t>Srebrne drzewo.</t>
+  </si>
+  <si>
+    <t>Król Vanyarów.</t>
+  </si>
+  <si>
+    <t>Pierwszy właściciel Huana.</t>
+  </si>
+  <si>
+    <t>Najbardziej wybuchowy syn Feaonra.</t>
+  </si>
+  <si>
+    <t>Zginął podczas trzeciego Bratobójstwa</t>
+  </si>
+  <si>
+    <t>Bliźniaczy brat Amroda.</t>
+  </si>
+  <si>
+    <t>Żona Feanora.</t>
+  </si>
+  <si>
+    <t>Został strącony w przepaść po zabójstwie żony.</t>
+  </si>
+  <si>
+    <t>Drzewo Numenoru.</t>
+  </si>
+  <si>
+    <t>Syn Elronda, przyjaciel Aragorna.</t>
+  </si>
+  <si>
+    <t>Dziadek Legolasa.</t>
+  </si>
+  <si>
+    <t>Królowa Rivendel.</t>
+  </si>
+  <si>
+    <t>Zabójca Throra.</t>
+  </si>
+  <si>
+    <t>Brat Galadrieli.</t>
+  </si>
+  <si>
+    <t>Zginął w bitwie Dagor Bragollach.</t>
+  </si>
+  <si>
+    <t>Odnaleziono tam Arcyklejnot.</t>
+  </si>
+  <si>
+    <t>Wschodni region Śródziemia.</t>
+  </si>
+  <si>
+    <t>Ukryte miasto.</t>
+  </si>
+  <si>
+    <t>Największa rzeka Beleriandu.</t>
+  </si>
+  <si>
+    <t>Pierwsza forteca Morgotha.</t>
+  </si>
+  <si>
+    <t>Siotra Thorina.</t>
+  </si>
+  <si>
+    <t>Królestwo rodu Durina.</t>
+  </si>
+  <si>
+    <t>Region zamieszkany przez Valarów.</t>
+  </si>
+  <si>
+    <t>Założony przez Dunedainów.</t>
+  </si>
+  <si>
+    <t>Twierdza w której ukrywał się Sauron, pod mianem Czarnoksiężnika.</t>
+  </si>
+  <si>
+    <t>Kraj Koni.</t>
+  </si>
+  <si>
+    <t>Rozbite pomiędzy braci.</t>
+  </si>
+  <si>
+    <t>Twierdza Saurona w Mordorze.</t>
+  </si>
+  <si>
+    <t>Inaczej Góra Przeznaczenia.</t>
+  </si>
+  <si>
+    <t>Córka Orodretha</t>
+  </si>
+  <si>
+    <t>Jego działania były bezpośrednią przyczyną upadku Numenoru.</t>
+  </si>
+  <si>
+    <t>Zabrano jej władzę.</t>
+  </si>
+  <si>
+    <t>Zginął podczas Bitwy Pięciu Armii. Dowódca Orków.</t>
+  </si>
+  <si>
+    <t>Nazywana Wieżą Czat.</t>
+  </si>
+  <si>
+    <t>Forteca opanowana przez Nazghule.</t>
+  </si>
+  <si>
+    <t>Drugi i ostatni Król Doriathu.</t>
+  </si>
+  <si>
+    <t>Eregion</t>
+  </si>
+  <si>
+    <t>Jego stolicą było Ost-in-Edhil.</t>
+  </si>
+  <si>
+    <t>Region wyzwolony od zła na koniec Trzeciej Ery.</t>
+  </si>
+  <si>
+    <t>Królestwo Elfów w Beleriandzie.</t>
+  </si>
+  <si>
+    <t>Kowale z tego miasta są odpowiedzialni za zabójstwo Króla.</t>
+  </si>
+  <si>
+    <t>Szary Pielgrzym</t>
+  </si>
+  <si>
+    <t>Rozbił ród królewski Numenoru.</t>
+  </si>
+  <si>
+    <t>Piąty Król Numenoru</t>
+  </si>
+  <si>
+    <t>Wolał podróżować niż rządzić.</t>
+  </si>
+  <si>
+    <t>Siostra Turina.</t>
+  </si>
+  <si>
+    <t>Odnalazł Arcyklejnot.</t>
+  </si>
+  <si>
+    <t>Jego kroniki zostały znalezione przez Drużynę Pierścienia w Morii.</t>
+  </si>
+  <si>
+    <t>Żelazna Stopa</t>
+  </si>
+  <si>
+    <t>Żelazny Dom</t>
+  </si>
+  <si>
+    <t>Zniszczone przez Smoka.</t>
+  </si>
+  <si>
+    <t>Miasto na wzgórzu Tuna.</t>
+  </si>
+  <si>
+    <t>Ojczyzna Froda.</t>
+  </si>
+  <si>
+    <t>Inaczej Nieśmiertelne Krainy.</t>
+  </si>
+  <si>
+    <t>Podbite przez okrów królestwo Krasnoludów.</t>
+  </si>
+  <si>
+    <t>Twierdza w cieniu szczytów Thangorodrimu.</t>
+  </si>
+  <si>
+    <t>Stolica Rohanu.</t>
+  </si>
+  <si>
+    <t>Twierdza była uważana jako "nie do zdobycia", póki chroniły jej ludzie.</t>
+  </si>
+  <si>
+    <t>Smok zabity przez Turina.</t>
+  </si>
+  <si>
+    <t>Władca Gondolinu.</t>
+  </si>
+  <si>
+    <t>Forteca Sarumana.</t>
+  </si>
+  <si>
+    <t>Miasto na jeziorze.</t>
+  </si>
+  <si>
+    <t>Stolica Arthedainu, zrujnowane przez Czarnoksiężnika z Angmaru.</t>
+  </si>
+  <si>
+    <t>Dosyć gruby krasnolud.</t>
+  </si>
+  <si>
+    <t>Jego Królem był Azaghal.</t>
+  </si>
+  <si>
+    <t>Niósł ze sobą olbrzymią odpowiedzialność.</t>
   </si>
 </sst>
 </file>
@@ -1189,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B168" sqref="B168"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1217,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1228,7 +1408,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1239,7 +1419,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1250,7 +1430,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1261,7 +1441,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1272,7 +1452,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1283,7 +1463,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1294,7 +1474,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1305,7 +1485,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1316,7 +1496,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1327,7 +1507,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1338,7 +1518,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1349,7 +1529,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1360,7 +1540,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1371,7 +1551,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1382,7 +1562,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1393,7 +1573,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1404,7 +1584,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1412,10 +1592,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1426,7 +1606,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1437,7 +1617,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1448,7 +1628,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1459,7 +1639,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1470,7 +1650,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1480,6 +1660,9 @@
       <c r="A26" t="s">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>333</v>
+      </c>
       <c r="C26">
         <v>0</v>
       </c>
@@ -1489,7 +1672,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1500,7 +1683,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1511,7 +1694,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1522,7 +1705,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1533,7 +1716,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1544,7 +1727,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1555,7 +1738,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1566,7 +1749,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1577,7 +1760,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1588,7 +1771,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1599,7 +1782,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1609,6 +1792,9 @@
       <c r="A38" t="s">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>259</v>
+      </c>
       <c r="C38">
         <v>0</v>
       </c>
@@ -1618,7 +1804,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1628,6 +1814,9 @@
       <c r="A40" t="s">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>260</v>
+      </c>
       <c r="C40">
         <v>0</v>
       </c>
@@ -1637,7 +1826,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1648,7 +1837,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1659,7 +1848,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1670,7 +1859,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>211</v>
+        <v>317</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1681,7 +1870,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1692,7 +1881,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1702,6 +1891,9 @@
       <c r="A47" t="s">
         <v>46</v>
       </c>
+      <c r="B47" t="s">
+        <v>261</v>
+      </c>
       <c r="C47">
         <v>0</v>
       </c>
@@ -1711,7 +1903,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1719,10 +1911,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B49" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1733,7 +1925,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1744,7 +1936,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1755,7 +1947,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1766,7 +1958,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1777,7 +1969,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1788,7 +1980,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1799,7 +1991,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1810,7 +2002,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1820,6 +2012,9 @@
       <c r="A58" t="s">
         <v>56</v>
       </c>
+      <c r="B58" t="s">
+        <v>264</v>
+      </c>
       <c r="C58">
         <v>0</v>
       </c>
@@ -1828,6 +2023,9 @@
       <c r="A59" t="s">
         <v>57</v>
       </c>
+      <c r="B59" t="s">
+        <v>262</v>
+      </c>
       <c r="C59">
         <v>0</v>
       </c>
@@ -1836,6 +2034,9 @@
       <c r="A60" t="s">
         <v>58</v>
       </c>
+      <c r="B60" t="s">
+        <v>263</v>
+      </c>
       <c r="C60">
         <v>0</v>
       </c>
@@ -1845,7 +2046,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1856,7 +2057,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1867,7 +2068,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1878,7 +2079,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1889,7 +2090,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1900,7 +2101,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1911,7 +2112,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1922,7 +2123,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1932,6 +2133,9 @@
       <c r="A69" t="s">
         <v>67</v>
       </c>
+      <c r="B69" t="s">
+        <v>265</v>
+      </c>
       <c r="C69">
         <v>0</v>
       </c>
@@ -1941,7 +2145,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1952,7 +2156,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1963,7 +2167,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1974,7 +2178,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1985,7 +2189,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -1995,6 +2199,9 @@
       <c r="A75" t="s">
         <v>73</v>
       </c>
+      <c r="B75" t="s">
+        <v>266</v>
+      </c>
       <c r="C75">
         <v>0</v>
       </c>
@@ -2004,7 +2211,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2015,7 +2222,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2026,7 +2233,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2037,7 +2244,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2047,6 +2254,9 @@
       <c r="A80" t="s">
         <v>78</v>
       </c>
+      <c r="B80" t="s">
+        <v>267</v>
+      </c>
       <c r="C80">
         <v>0</v>
       </c>
@@ -2055,6 +2265,9 @@
       <c r="A81" t="s">
         <v>79</v>
       </c>
+      <c r="B81" t="s">
+        <v>268</v>
+      </c>
       <c r="C81">
         <v>0</v>
       </c>
@@ -2063,6 +2276,9 @@
       <c r="A82" t="s">
         <v>80</v>
       </c>
+      <c r="B82" t="s">
+        <v>269</v>
+      </c>
       <c r="C82">
         <v>0</v>
       </c>
@@ -2071,6 +2287,9 @@
       <c r="A83" t="s">
         <v>81</v>
       </c>
+      <c r="B83" t="s">
+        <v>270</v>
+      </c>
       <c r="C83">
         <v>0</v>
       </c>
@@ -2079,6 +2298,9 @@
       <c r="A84" t="s">
         <v>82</v>
       </c>
+      <c r="B84" t="s">
+        <v>271</v>
+      </c>
       <c r="C84">
         <v>0</v>
       </c>
@@ -2088,7 +2310,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2098,6 +2320,9 @@
       <c r="A86" t="s">
         <v>84</v>
       </c>
+      <c r="B86" t="s">
+        <v>272</v>
+      </c>
       <c r="C86">
         <v>0</v>
       </c>
@@ -2106,6 +2331,9 @@
       <c r="A87" t="s">
         <v>85</v>
       </c>
+      <c r="B87" t="s">
+        <v>273</v>
+      </c>
       <c r="C87">
         <v>0</v>
       </c>
@@ -2114,13 +2342,19 @@
       <c r="A88" t="s">
         <v>86</v>
       </c>
+      <c r="B88" t="s">
+        <v>274</v>
+      </c>
       <c r="C88">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>275</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2128,7 +2362,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>226</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2136,10 +2373,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>240</v>
+        <v>281</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2147,7 +2384,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>282</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2155,7 +2395,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>297</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2163,7 +2406,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>303</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -2171,7 +2417,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>276</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -2179,7 +2428,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>277</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -2187,7 +2439,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>278</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -2195,7 +2450,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>279</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -2203,7 +2461,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>298</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -2211,7 +2472,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>87</v>
+      </c>
+      <c r="B100" t="s">
+        <v>299</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -2221,6 +2485,9 @@
       <c r="A101" t="s">
         <v>99</v>
       </c>
+      <c r="B101" t="s">
+        <v>280</v>
+      </c>
       <c r="C101">
         <v>0</v>
       </c>
@@ -2229,6 +2496,9 @@
       <c r="A102" t="s">
         <v>100</v>
       </c>
+      <c r="B102" t="s">
+        <v>300</v>
+      </c>
       <c r="C102">
         <v>0</v>
       </c>
@@ -2237,6 +2507,9 @@
       <c r="A103" t="s">
         <v>101</v>
       </c>
+      <c r="B103" t="s">
+        <v>246</v>
+      </c>
       <c r="C103">
         <v>0</v>
       </c>
@@ -2245,6 +2518,9 @@
       <c r="A104" t="s">
         <v>102</v>
       </c>
+      <c r="B104" t="s">
+        <v>301</v>
+      </c>
       <c r="C104">
         <v>0</v>
       </c>
@@ -2254,7 +2530,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -2262,7 +2538,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>304</v>
+      </c>
+      <c r="B106" t="s">
+        <v>305</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -2270,7 +2549,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="B107" t="s">
+        <v>247</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -2278,7 +2560,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="B108" t="s">
+        <v>292</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -2286,10 +2571,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>261</v>
+        <v>293</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -2297,7 +2582,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="B110" t="s">
+        <v>291</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -2305,7 +2593,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="B111" t="s">
+        <v>294</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -2313,7 +2604,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="B112" t="s">
+        <v>248</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -2321,7 +2615,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="B113" t="s">
+        <v>283</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2329,10 +2626,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>262</v>
+        <v>284</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -2340,7 +2637,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="B115" t="s">
+        <v>306</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -2348,7 +2648,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="B116" t="s">
+        <v>296</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -2356,7 +2659,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+      <c r="B117" t="s">
+        <v>295</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -2364,7 +2670,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="B118" t="s">
+        <v>249</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -2372,7 +2681,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="B119" t="s">
+        <v>250</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -2380,10 +2692,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>263</v>
+        <v>307</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -2391,10 +2703,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -2402,7 +2714,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="B122" t="s">
+        <v>285</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -2410,10 +2725,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -2421,7 +2736,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="B124" t="s">
+        <v>286</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -2429,10 +2747,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -2440,7 +2758,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="B126" t="s">
+        <v>288</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -2448,7 +2769,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="B127" t="s">
+        <v>332</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -2456,7 +2780,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="B128" t="s">
+        <v>308</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -2464,7 +2791,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="B129" t="s">
+        <v>253</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -2472,7 +2802,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B130" t="s">
+        <v>289</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -2480,10 +2813,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -2491,7 +2824,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="B132" t="s">
+        <v>290</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2499,10 +2835,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" t="s">
-        <v>268</v>
+        <v>320</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -2510,7 +2846,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="B134" t="s">
+        <v>321</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -2518,7 +2857,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="B135" t="s">
+        <v>322</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -2526,7 +2868,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="B136" t="s">
+        <v>318</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -2534,7 +2879,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="B137" t="s">
+        <v>323</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -2542,7 +2890,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="B138" t="s">
+        <v>328</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -2550,7 +2901,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="B139" t="s">
+        <v>319</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -2558,7 +2912,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="B140" t="s">
+        <v>255</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -2566,10 +2923,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" t="s">
-        <v>269</v>
+        <v>200</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -2577,10 +2934,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" t="s">
-        <v>270</v>
+        <v>324</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -2588,7 +2945,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="B143" t="s">
+        <v>329</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -2596,7 +2956,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="B144" t="s">
+        <v>330</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -2604,7 +2967,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="B145" t="s">
+        <v>325</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -2612,7 +2978,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="B146" t="s">
+        <v>256</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -2620,7 +2989,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="B147" t="s">
+        <v>326</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -2628,7 +3000,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="B148" t="s">
+        <v>327</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -2636,10 +3011,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" t="s">
-        <v>271</v>
+        <v>331</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -2647,7 +3022,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="B150" t="s">
+        <v>258</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -2655,7 +3033,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>148</v>
+      </c>
+      <c r="B151" t="s">
+        <v>257</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -2663,7 +3044,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="B152" t="s">
+        <v>315</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -2671,7 +3055,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>150</v>
+      </c>
+      <c r="B153" t="s">
+        <v>316</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -2679,10 +3066,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B154" t="s">
-        <v>273</v>
+        <v>314</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -2690,7 +3077,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="B155" t="s">
+        <v>313</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -2701,7 +3091,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -2711,6 +3101,9 @@
       <c r="A157" t="s">
         <v>155</v>
       </c>
+      <c r="B157" t="s">
+        <v>310</v>
+      </c>
       <c r="C157">
         <v>0</v>
       </c>
@@ -2719,6 +3112,9 @@
       <c r="A158" t="s">
         <v>156</v>
       </c>
+      <c r="B158" t="s">
+        <v>311</v>
+      </c>
       <c r="C158">
         <v>0</v>
       </c>
@@ -2727,6 +3123,9 @@
       <c r="A159" t="s">
         <v>157</v>
       </c>
+      <c r="B159" t="s">
+        <v>312</v>
+      </c>
       <c r="C159">
         <v>0</v>
       </c>
@@ -2735,6 +3134,9 @@
       <c r="A160" t="s">
         <v>158</v>
       </c>
+      <c r="B160" t="s">
+        <v>232</v>
+      </c>
       <c r="C160">
         <v>0</v>
       </c>
@@ -2743,6 +3145,9 @@
       <c r="A161" t="s">
         <v>159</v>
       </c>
+      <c r="B161" t="s">
+        <v>227</v>
+      </c>
       <c r="C161">
         <v>0</v>
       </c>
@@ -2751,6 +3156,9 @@
       <c r="A162" t="s">
         <v>160</v>
       </c>
+      <c r="B162" t="s">
+        <v>309</v>
+      </c>
       <c r="C162">
         <v>0</v>
       </c>
@@ -2759,6 +3167,9 @@
       <c r="A163" t="s">
         <v>161</v>
       </c>
+      <c r="B163" t="s">
+        <v>231</v>
+      </c>
       <c r="C163">
         <v>0</v>
       </c>
@@ -2767,13 +3178,19 @@
       <c r="A164" t="s">
         <v>162</v>
       </c>
+      <c r="B164" t="s">
+        <v>230</v>
+      </c>
       <c r="C164">
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>217</v>
+      </c>
+      <c r="B165" t="s">
+        <v>229</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -2781,7 +3198,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>218</v>
+      </c>
+      <c r="B166" t="s">
+        <v>228</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -2789,121 +3209,13 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>166</v>
+        <v>235</v>
       </c>
       <c r="B167" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C167">
         <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
-        <v>167</v>
-      </c>
-      <c r="C168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
-        <v>168</v>
-      </c>
-      <c r="C169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
-        <v>169</v>
-      </c>
-      <c r="C170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
-        <v>170</v>
-      </c>
-      <c r="C171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>171</v>
-      </c>
-      <c r="B172" t="s">
-        <v>246</v>
-      </c>
-      <c r="C172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>172</v>
-      </c>
-      <c r="B173" t="s">
-        <v>241</v>
-      </c>
-      <c r="C173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
-        <v>173</v>
-      </c>
-      <c r="C174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
-        <v>174</v>
-      </c>
-      <c r="B175" t="s">
-        <v>245</v>
-      </c>
-      <c r="C175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
-        <v>175</v>
-      </c>
-      <c r="B176" t="s">
-        <v>244</v>
-      </c>
-      <c r="C176">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
-        <v>231</v>
-      </c>
-      <c r="B177" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
-        <v>232</v>
-      </c>
-      <c r="B178" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
-        <v>249</v>
-      </c>
-      <c r="B179" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>